<commit_message>
:up: flashcards mais estilizados
</commit_message>
<xml_diff>
--- a/banco_de_dados/flashcards.xlsx
+++ b/banco_de_dados/flashcards.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="flashcards" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,6 +458,41 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Gestão da Qualidade</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>processos universais da Trilogia de Juran</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>&lt;ul&gt;
+&lt;li&gt;Planejamento da Qualidade&lt;/li&gt;
+&lt;li&gt;Controle da Qualidade&lt;/li&gt;
+&lt;li&gt;Melhoria da Qualidade&lt;/li&gt;
+&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:up: ultimo commit antes de tentar fazer aparecer varios cartoes de uma so vez
</commit_message>
<xml_diff>
--- a/banco_de_dados/flashcards.xlsx
+++ b/banco_de_dados/flashcards.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,6 +493,47 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Gestão da Qualidade</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Trilogia Juran&lt;/b&gt;
+Planejamento da qualidade</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>&lt;ul&gt;
+	&lt;li&gt;Planejamento da qualidade&lt;/li&gt;
+&lt;/ul&gt;
+&lt;b&gt;são estabelecidos:&lt;/b&gt;
+&lt;ul&gt;
+	&lt;li&gt;objetivos&lt;/li&gt;
+	&lt;li&gt;planos de ação&lt;/li&gt;
+	&lt;li&gt;bem como metas de qualidade&lt;/li&gt;
+	&lt;li&gt;os produtos e processos necessários à realização dessas metas&lt;/li&gt;
+&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:up: melhoria no design dos flashcardas
</commit_message>
<xml_diff>
--- a/banco_de_dados/flashcards.xlsx
+++ b/banco_de_dados/flashcards.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,6 +534,76 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Gestão da Qualidade</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Trilogia Juran&lt;/b&gt;&lt;br&gt;
+Controle da Qualidade</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>&lt;ul&gt;
+	&lt;li&gt;inspeções contínuas para garantir que os processos estejam sob controle&lt;/li&gt;
+	&lt;li&gt;fazer um comparativo entre o desempenho real e o desempenho planejado&lt;/li&gt;
+&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Gestão da Qualidade</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Trilogia Juran&lt;/b&gt;&lt;br&gt;
+Melhoria da qualidade</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>&lt;ul&gt;
+	&lt;li&gt;refinamento proativo dos processos para melhorá-los&lt;/li&gt;
+	&lt;li&gt;aprimorar o desempenho rumo a um nível superior de qualidade&lt;/li&gt;
+&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:lady_beetle: espaçamento excessivo nos backs dos cartoes resolvido
</commit_message>
<xml_diff>
--- a/banco_de_dados/flashcards.xlsx
+++ b/banco_de_dados/flashcards.xlsx
@@ -494,8 +494,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -515,16 +517,18 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>&lt;ul&gt;
-	&lt;li&gt;Planejamento da qualidade&lt;/li&gt;
-&lt;/ul&gt;
-&lt;b&gt;são estabelecidos:&lt;/b&gt;
+          <t xml:space="preserve">&lt;ul&gt;
+&lt;li&gt;A etapa de desing&lt;/li&gt;
+&lt;li&gt;são estabelecidos:
 &lt;ul&gt;
 	&lt;li&gt;objetivos&lt;/li&gt;
 	&lt;li&gt;planos de ação&lt;/li&gt;
 	&lt;li&gt;bem como metas de qualidade&lt;/li&gt;
 	&lt;li&gt;os produtos e processos necessários à realização dessas metas&lt;/li&gt;
-&lt;/ul&gt;</t>
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;
+</t>
         </is>
       </c>
       <c r="F3" t="n">

</xml_diff>

<commit_message>
:package: modo cego adicionado em praticar \n:package: comentários adicionado no db \n:package: modo escuro adicionado;\n:package: flascard dinamico adicionado nas questoes erradas em praticar
</commit_message>
<xml_diff>
--- a/banco_de_dados/flashcards.xlsx
+++ b/banco_de_dados/flashcards.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -608,6 +608,41 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Matemática Básica</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Operações</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Tabuada de multiplicação de 6 a 8</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>&lt;ul&gt;
+	&lt;li&gt;6 x 7 = 42&lt;/li&gt;
+	&lt;li&gt;6 x 8 = 48&lt;/li&gt;
+	&lt;li&gt;7 x 8 = 56&lt;/li&gt;
+&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:package: botão de rederizar previa de questao no preview done
</commit_message>
<xml_diff>
--- a/banco_de_dados/flashcards.xlsx
+++ b/banco_de_dados/flashcards.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -643,6 +643,33 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Estatística</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Distribuições Conjuntas e Momentos de Variáveis Aleatórias</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Estudar coeficiente de correlação</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:up: algumas questoes respondidas
</commit_message>
<xml_diff>
--- a/banco_de_dados/flashcards.xlsx
+++ b/banco_de_dados/flashcards.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -643,33 +643,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Estatística</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Distribuições Conjuntas e Momentos de Variáveis Aleatórias</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Estudar coeficiente de correlação</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:up: pequenos ajustes nos flashcards
</commit_message>
<xml_diff>
--- a/banco_de_dados/flashcards.xlsx
+++ b/banco_de_dados/flashcards.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -643,6 +643,79 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Gestão da Produção e Operações</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">&lt;b&gt;ASPECTOS HISTÓRICOS E EVOLUTIVOS&lt;/b&gt;
+do:
+&lt;ul&gt;
+	&lt;li&gt;&lt;b&gt;MRP I&lt;/b&gt;&lt;/li&gt;
+	&lt;li&gt;&lt;b&gt;MRP II&lt;/b&gt;&lt;/li&gt;
+	&lt;li&gt;&lt;b&gt;ERP I&lt;/b&gt;&lt;/li&gt;
+	&lt;li&gt;&lt;b&gt;ERP II&lt;/b&gt;&lt;/li&gt;
+	&lt;li&gt;&lt;b&gt;ERPs baseados em nuvem (SaaS)&lt;/b&gt;&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>&lt;ul&gt;
+	&lt;li&gt;&lt;b&gt;MRP I:&lt;/b&gt;
+&lt;ul&gt;
+	&lt;li&gt;Foco no planejamento de materiais necessários para a produção;&lt;/li&gt;
+	&lt;li&gt;Estrutura baseada em listas de materiais (BOM – Bill of Materials), programação de ordens de&lt;/li&gt;
+	&lt;li&gt;compra e produção;&lt;/li&gt;
+	&lt;li&gt;Objetivo central: minimizar estoques e garantir disponibilidade de insumos.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+	&lt;li&gt;&lt;b&gt;MRP II&lt;/b&gt;
+&lt;ul&gt;
+	&lt;li&gt;Expansão do MRP para incluir capacidade produtiva, finanças e simulações;&lt;/li&gt;
+	&lt;li&gt;Incorporação de planejamento financeiro integrado com o plano mestre de produção;&lt;/li&gt;
+	&lt;li&gt;Primeiro movimento em direção à integração interfuncional.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+	&lt;li&gt;&lt;b&gt;ERP I&lt;/b&gt;
+&lt;ul&gt;
+	&lt;li&gt;Integração total de todos os departamentos e funções empresariais;&lt;/li&gt;
+	&lt;li&gt;Inclusão de módulos de vendas, distribuição, contabilidade, RH, manutenção e outros;&lt;/li&gt;
+	&lt;li&gt;Capacidade de operar em ambientes multiempresa e multinacionais.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+	&lt;li&gt;&lt;b&gt;ERP II&lt;/b&gt;
+&lt;ul&gt;
+	&lt;li&gt;com integração entre empresas via internet e cadeia de suprimentos (SCM).&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+	&lt;li&gt;&lt;b&gt;ERPs baseados em nuvem (SaaS)&lt;/b&gt;
+&lt;ul&gt;
+	&lt;li&gt;que ampliam escalabilidade e flexibilidade.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
+&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:up: pequenos ajustes nos flashcards - p2
</commit_message>
<xml_diff>
--- a/banco_de_dados/flashcards.xlsx
+++ b/banco_de_dados/flashcards.xlsx
@@ -644,8 +644,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -676,34 +678,41 @@
           <t>&lt;ul&gt;
 	&lt;li&gt;&lt;b&gt;MRP I:&lt;/b&gt;
 &lt;ul&gt;
-	&lt;li&gt;Foco no planejamento de materiais necessários para a produção;&lt;/li&gt;
-	&lt;li&gt;Estrutura baseada em listas de materiais (BOM – Bill of Materials), programação de ordens de&lt;/li&gt;
-	&lt;li&gt;compra e produção;&lt;/li&gt;
-	&lt;li&gt;Objetivo central: minimizar estoques e garantir disponibilidade de insumos.&lt;/li&gt;
+&lt;li&gt;décadas de 1960–1970&lt;/li&gt;
+	&lt;li&gt;Planejamento de materiais;&lt;/li&gt;
+	&lt;li&gt;BOM – Bill of Materials, programação de ordens;&lt;/li&gt;
+	&lt;li&gt;Objetivo central:
+&lt;ul&gt;
+	&lt;li&gt;minimizar estoques&lt;/li&gt;
+	&lt;li&gt;garantir disponibilidade de insumos.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/li&gt;
 &lt;/ul&gt;
 &lt;/li&gt;
 	&lt;li&gt;&lt;b&gt;MRP II&lt;/b&gt;
 &lt;ul&gt;
-	&lt;li&gt;Expansão do MRP para incluir capacidade produtiva, finanças e simulações;&lt;/li&gt;
-	&lt;li&gt;Incorporação de planejamento financeiro integrado com o plano mestre de produção;&lt;/li&gt;
-	&lt;li&gt;Primeiro movimento em direção à integração interfuncional.&lt;/li&gt;
+&lt;li&gt;décadas de 1970–1980&lt;/li&gt;
+	&lt;li&gt;capacidade produtiva, finanças e simulações;&lt;/li&gt;
+	&lt;li&gt;planejamento financeiro integrado;&lt;/li&gt;
+	&lt;li&gt;integração interfuncional.&lt;/li&gt;
 &lt;/ul&gt;
 &lt;/li&gt;
 	&lt;li&gt;&lt;b&gt;ERP I&lt;/b&gt;
 &lt;ul&gt;
-	&lt;li&gt;Integração total de todos os departamentos e funções empresariais;&lt;/li&gt;
-	&lt;li&gt;Inclusão de módulos de vendas, distribuição, contabilidade, RH, manutenção e outros;&lt;/li&gt;
-	&lt;li&gt;Capacidade de operar em ambientes multiempresa e multinacionais.&lt;/li&gt;
+&lt;li&gt;década de 1990 em diante&lt;/li&gt;
+	&lt;li&gt;total de todos os departamentos e funções;&lt;/li&gt;
+	&lt;li&gt;módulos de vendas, distribuição, contabilidade, RH, manutenção e outros;&lt;/li&gt;
+	&lt;li&gt;ambientes multiempresa e multinacionais.&lt;/li&gt;
 &lt;/ul&gt;
 &lt;/li&gt;
 	&lt;li&gt;&lt;b&gt;ERP II&lt;/b&gt;
 &lt;ul&gt;
-	&lt;li&gt;com integração entre empresas via internet e cadeia de suprimentos (SCM).&lt;/li&gt;
+	&lt;li&gt;integração entre empresas via internet e cadeia de suprimentos (SCM).&lt;/li&gt;
 &lt;/ul&gt;
 &lt;/li&gt;
 	&lt;li&gt;&lt;b&gt;ERPs baseados em nuvem (SaaS)&lt;/b&gt;
 &lt;ul&gt;
-	&lt;li&gt;que ampliam escalabilidade e flexibilidade.&lt;/li&gt;
+	&lt;li&gt;ampliam escalabilidade e flexibilidade.&lt;/li&gt;
 &lt;/ul&gt;
 &lt;/li&gt;
 &lt;/ul&gt;</t>
@@ -713,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:up: pequenos ajustes nos flashcards - p3
</commit_message>
<xml_diff>
--- a/banco_de_dados/flashcards.xlsx
+++ b/banco_de_dados/flashcards.xlsx
@@ -490,7 +490,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -535,7 +535,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -570,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -605,7 +605,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -722,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:up: plano de estudos melhorado (vizualização), algumas questoes respondidas
</commit_message>
<xml_diff>
--- a/banco_de_dados/flashcards.xlsx
+++ b/banco_de_dados/flashcards.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2926,6 +2926,563 @@
         <v>0</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Conceito de Logística (&lt;i&gt;Council of Logistics Management&lt;/i&gt;):</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>é o processo de controle, planejamento e implementação do fluxo</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>objetivo da logística, Ballou (2005):</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>dispor a mercadoria ou o serviço certo, no lugar certo, no tempo certo e nas condições desejadas</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>tripé logístico</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>&lt;ul&gt;
+	&lt;li&gt;Transporte;&lt;/li&gt;
+	&lt;li&gt;Distribuição; e&lt;/li&gt;
+	&lt;li&gt;Armazenagem.&lt;/li&gt;
+&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>divisão da logística segundo algumas literaturas</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>&lt;ul&gt;
+	&lt;li&gt;Atividades primárias: &lt;ul&gt; &lt;li&gt;Transportes,&lt;/li&gt; &lt;li&gt;Processamento de Pedidos e&lt;/li&gt; &lt;li&gt;Manutenção de estoques;&lt;/li&gt; &lt;/ul&gt; &lt;i&gt;Minemônico (TPM)&lt;/i&gt;&lt;/li&gt;
+	&lt;li&gt;Atividades de apoio: &lt;ul&gt; &lt;li&gt;Armazenagem,&lt;/li&gt; &lt;li&gt;Manuseio de Materiais,&lt;/li&gt; &lt;li&gt;Embalagem de Proteção,&lt;/li&gt; &lt;li&gt;Obtenção, Programação de Produtos e&lt;/li&gt; &lt;li&gt;Manutenção de Informação.&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Processo de fluxo de materias:</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>&lt;ol&gt;
+	&lt;li&gt;Entradas - Fornecedores&lt;/li&gt;
+	&lt;li&gt;Estoque/Arm azenamento&lt;/li&gt;
+	&lt;li&gt;Processo Produtivo&lt;/li&gt;
+	&lt;li&gt;Produtos acabados (depósito)&lt;/li&gt;
+	&lt;li&gt;Saídas - Clientes&lt;/li&gt;
+&lt;/ol&gt;</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Classe de materiais ao longo do processo produtivo</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>&lt;ul&gt;
+	&lt;li&gt;Matéria-prima&lt;/li&gt;
+	&lt;li&gt;Materiais em processamento&lt;/li&gt;
+	&lt;li&gt;Materiais semiacabados&lt;/li&gt;
+	&lt;li&gt;Materiais acabados&lt;/li&gt;
+	&lt;li&gt;Produtos acabados&lt;/li&gt;
+&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Transporte:&lt;/b&gt;
+&lt;i&gt;Características&lt;/i&gt;</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Conceito: &lt;ul&gt; &lt;li&gt;parte do processo logístico responsável por levar os produtos ao consumidor final e/ou entre fornecedor e produtor&lt;/li&gt; &lt;/ul&gt;
+corresponde, em média, a 2/3 de todo o custo logístico
+fatores determinantes em relação ao transporte é a escolha do modal: &lt;ul&gt; &lt;li&gt;Custo do transporte;&lt;/li&gt; &lt;li&gt;Velocidade com que o produto é transportado;&lt;/li&gt; &lt;li&gt;Tipo de manuseio do produto durante o transporte; e&lt;/li&gt; &lt;li&gt;Quantidade de viagens&lt;/li&gt; &lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Modais de Transporte:</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">&lt;ul&gt; &lt;li&gt;&lt;b&gt;Aeroviário &lt;/b&gt;&lt;ul&gt; &lt;li&gt;Vantages: &lt;ul&gt; &lt;li&gt;longas distâncias, independente da geografia&lt;/li&gt; &lt;li&gt;mais rápido dentre os modais&lt;/li&gt; &lt;li&gt;Menor custo com embalagens&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;li&gt;desvantagens: &lt;ul&gt; &lt;li&gt;volume pequeno&lt;/li&gt; &lt;li&gt;custo mais elevado&lt;/li&gt; &lt;li&gt;geralmente precisa de outro modal para concluir o transporte&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;li&gt;&lt;b&gt;Aquaviário &lt;/b&gt;&lt;ul&gt; &lt;li&gt;&lt;b&gt;Marítimo:&lt;/b&gt; mares e oceanos&lt;/li&gt; &lt;li&gt;&lt;b&gt;Fluvial:&lt;/b&gt; rios&lt;/li&gt; &lt;li&gt;&lt;b&gt;Lacustre:&lt;/b&gt; lagos e lagoas.&lt;/li&gt; &lt;li&gt;vantagens: &lt;ul&gt; &lt;li&gt;Maior capacidade de carga entre os modais;&lt;/li&gt; &lt;li&gt;grandes distâncias de forma autônoma&lt;/li&gt; &lt;li&gt;Baixo custo unitário de carregamento&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;li&gt;desvantagens: &lt;ul&gt; &lt;li&gt;mais lento entre os modais;&lt;/li&gt; &lt;li&gt;Maior suscetibilidade as mudanças da natureza;&lt;/li&gt; &lt;li&gt;Necessidade de terminais especializados&lt;/li&gt; &lt;li&gt;Desembaraço burocrático&lt;/li&gt; &lt;li&gt;Alto custo quanto ao seguro&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;li&gt;&lt;b&gt;Ferroviário &lt;/b&gt;&lt;ul&gt; &lt;li&gt;vantagens: &lt;ul&gt; &lt;li&gt;Baixo custo&lt;/li&gt; &lt;li&gt;Menor risco de acidentes&lt;/li&gt; &lt;li&gt;grande capacidade&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;li&gt;desvantagens: &lt;ul&gt; &lt;li&gt;geralmente precisa de outro modal para concluir o transporte&lt;/li&gt; &lt;li&gt;Baixo investimento governamental&lt;/li&gt; &lt;li&gt;Rotas fixas e inflexíveis&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;li&gt;&lt;b&gt;Rodoviário&lt;/b&gt; &lt;ul&gt; &lt;li&gt;vantagens: &lt;ul&gt; &lt;li&gt;acessibilidade&lt;/li&gt; &lt;li&gt;Rapidez para contratação&lt;/li&gt; &lt;li&gt;Rotas flexíveis&lt;/li&gt; &lt;li&gt;Menor burocracia entre os modais&lt;/li&gt; &lt;li&gt;Menor custo de estrutura e alto investimento gorvenamental&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;li&gt;desvantagens: &lt;ul&gt; &lt;li&gt;Gastos com pedágio&lt;/li&gt; &lt;li&gt;aumento de combustíveis tendem a aumentar o valor do frete&lt;/li&gt; &lt;li&gt;capacidade de carga é bem menor&lt;/li&gt; &lt;li&gt;baixa autonomia de deslocamento&lt;/li&gt; &lt;li&gt;Maior chance de extravio&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;li&gt;&lt;b&gt;Dutoviário &lt;/b&gt;&lt;ul&gt; &lt;li&gt;vantagens: &lt;ul&gt; &lt;li&gt;transporta grande volume de carga de forma constante&lt;/li&gt; &lt;li&gt;grande confiabilidade no processo&lt;/li&gt; &lt;li&gt;Baixos custos operacionais;&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;li&gt;Desvantagens: &lt;ul&gt; &lt;li&gt;Custo inicial para implantação altíssimo&lt;/li&gt; &lt;li&gt;Burocracia ambiental&lt;/li&gt; &lt;li&gt;Reduzida flexibilidade de trajeto.&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;/ul&gt;
+</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Classificação dos Modais:</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>&lt;ul&gt; &lt;li&gt;&lt;b&gt;Velocidade de Transporte:&lt;/b&gt; &lt;ol&gt; &lt;li&gt;Aeroviário&lt;/li&gt; &lt;li&gt;Rodoviário&lt;/li&gt; &lt;li&gt;Ferroviário&lt;/li&gt; &lt;li&gt;Aquaviário&lt;/li&gt; &lt;li&gt;Dutoviário&lt;/li&gt; &lt;/ol&gt;&lt;/li&gt; &lt;li&gt;&lt;b&gt;Disponibilidade:&lt;/b&gt; &lt;ol&gt; &lt;li&gt;Rodoviário&lt;/li&gt; &lt;li&gt;Ferroviário&lt;/li&gt; &lt;li&gt;Aeroviário&lt;/li&gt; &lt;li&gt;Aquaviário&lt;/li&gt; &lt;li&gt;Dutoviário&lt;/li&gt; &lt;/ol&gt;&lt;/li&gt; &lt;li&gt;&lt;b&gt;Confiabilidade: &lt;/b&gt;&lt;ol&gt; &lt;li&gt;Dutoviário&lt;/li&gt; &lt;li&gt;Rodoviário&lt;/li&gt; &lt;li&gt;Ferroviário&lt;/li&gt; &lt;li&gt;Aquaviário&lt;/li&gt; &lt;li&gt;Aeroviário&lt;/li&gt; &lt;/ol&gt;&lt;/li&gt; &lt;li&gt;&lt;b&gt;Capacidade de Carga:&lt;/b&gt; &lt;ol&gt; &lt;li&gt;Aquaviário&lt;/li&gt; &lt;li&gt;Ferroviário&lt;/li&gt; &lt;li&gt;Rodoviário&lt;/li&gt; &lt;li&gt;Aeroviário&lt;/li&gt; &lt;li&gt;Dutoviário&lt;/li&gt; &lt;/ol&gt;&lt;/li&gt; &lt;li&gt;&lt;b&gt;Frequência:&lt;/b&gt; &lt;ol&gt; &lt;li&gt;Dutoviário&lt;/li&gt; &lt;li&gt;Rodoviário&lt;/li&gt; &lt;li&gt;Aeroviário&lt;/li&gt; &lt;li&gt;Ferroviário&lt;/li&gt; &lt;li&gt;Aquaviário&lt;/li&gt; &lt;/ol&gt;&lt;/li&gt; &lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Distribuição&lt;/b&gt;
+&lt;i&gt;Características&lt;/i&gt;</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">&lt;ul&gt;
+	&lt;li&gt;&lt;b&gt;Caonceito:&lt;/b&gt; &lt;ul&gt; &lt;li&gt;conjunto de ações voltadas à gestão de materiais, iniciando com a saída do produto do processo produtivo e terminando com a entrega no ponto final de consumo&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+	&lt;li&gt;&lt;b&gt;fatores mais importantes ligados à distribuição&lt;/b&gt; &lt;ul&gt; &lt;li&gt;Conferência de cargas;&lt;/li&gt; &lt;li&gt;Gestão do frete;&lt;/li&gt; &lt;li&gt;Gestão do transporte;&lt;/li&gt; &lt;li&gt;Análise e desempenho de indicadores;&lt;/li&gt; &lt;li&gt;Gestão de Rotas ou Roteirização.&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Armazenamento&lt;/b&gt;
+&lt;i&gt;Características&lt;/i&gt;</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>&lt;ul&gt;
+	&lt;li&gt;atividades que compreende a armazenagem: &lt;ul&gt; &lt;li&gt;receber&lt;/li&gt; &lt;li&gt;carregar&lt;/li&gt; &lt;li&gt;descarregar&lt;/li&gt; &lt;li&gt;conservar&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+	&lt;li&gt;quatro pontos principais para que uma empresa decida destinar uma parte de sua área útil à armazenagem, Ballou (1993): &lt;ul&gt; &lt;li&gt;reduzir custos de transporte e produção&lt;/li&gt; &lt;li&gt;coordenação de suprimento e demanda&lt;/li&gt; &lt;li&gt;auxílio ao processo de produção&lt;/li&gt; &lt;li&gt;&lt;u&gt;auxílio ao processo de marketing.&lt;/u&gt;&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+	&lt;li&gt;funções da armazenagem, Ballou (1993): &lt;ul&gt; &lt;li&gt;Abrigo de produtos&lt;/li&gt; &lt;li&gt;Consolidação&lt;/li&gt; &lt;li&gt;Transferência e Transbordo&lt;/li&gt; &lt;li&gt;Agrupamento&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+	&lt;li&gt;&lt;b&gt;codificação:&lt;/b&gt; &lt;ul&gt; &lt;li&gt;catalogar, simplificar, especificar, normatizar e padronizar todo o estoque&lt;/li&gt; &lt;li&gt;11 dígitos: &lt;ol&gt; &lt;li&gt;XX - Grupo&lt;/li&gt; &lt;li&gt;XX - Classe&lt;/li&gt; &lt;li&gt;XXXXXX - Código de identificação&lt;/li&gt; &lt;li&gt;X - Dígito de Controle&lt;/li&gt; &lt;/ol&gt;&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+	&lt;li&gt;&lt;b&gt;embalagens:&lt;/b&gt; &lt;ul&gt; &lt;li&gt;vantagens: &lt;ul&gt; &lt;li&gt;proteção ao produto &lt;ul&gt; &lt;li&gt;manuseio&lt;/li&gt; &lt;li&gt;transporte&lt;/li&gt; &lt;li&gt;armazenagem&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+	&lt;li&gt;ações pelos quais passam os materiais armazenados: &lt;ul&gt; &lt;li&gt;Especificação&lt;/li&gt; &lt;li&gt;Simplificação&lt;/li&gt; &lt;li&gt;Codificação&lt;/li&gt; &lt;li&gt;Padronização&lt;/li&gt; &lt;li&gt;Catalogação&lt;/li&gt; &lt;li&gt;Normalização&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+	&lt;li&gt;&lt;b&gt;sistemas de armazenamento:&lt;/b&gt; &lt;ul&gt; &lt;li&gt;Sistema WMS&lt;/li&gt; &lt;li&gt;Racks&lt;/li&gt; &lt;li&gt;Mezanino&lt;/li&gt; &lt;li&gt;Sistema de carrossel&lt;/li&gt; &lt;li&gt;Porta-paletes&lt;/li&gt; &lt;li&gt;Flow Rack&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Sistemas Logísticos</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>&lt;ul&gt;
+	&lt;li&gt;TMS&lt;/li&gt;
+	&lt;li&gt;WMS&lt;/li&gt;
+	&lt;li&gt;Sistema de monitoramento de cargas&lt;/li&gt;
+	&lt;li&gt;Sistemas de roteirização&lt;/li&gt;
+	&lt;li&gt;Sistemas de gestão de frotas.&lt;/li&gt;
+&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Logística Reversa&lt;/b&gt;
+&lt;i&gt;Características&lt;/i&gt;</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>&lt;ul&gt;
+	&lt;li&gt;responsabilidade sobre os resíduos produzidos em decorrência do consumo de bens&lt;/li&gt;
+	&lt;li&gt;devolução, reciclagem e adequada destinação de produtos pós-venda e pós consumo.&lt;/li&gt;
+	&lt;li&gt;etapas: &lt;ol&gt; &lt;li&gt;Devolução da embalagem ou resíduo para o comerciante;&lt;/li&gt; &lt;li&gt;O comerciante devolve para ao fabricante; e&lt;/li&gt; &lt;li&gt;O fabricante destina para reuso, reciclagem ou descarte adequado.&lt;/li&gt; &lt;/ol&gt;&lt;/li&gt;
+	&lt;li&gt;leis que devem ser cumpridas&lt;/li&gt;
+	&lt;li&gt;preocupação com a lucratividade e sustentabilidade desse processo&lt;/li&gt;
+	&lt;li&gt;reversa: &lt;ul&gt; &lt;li&gt;transporte dos produtos nas mãos dos clientes de volta para a empresa&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+	&lt;li&gt;atividades: &lt;ul&gt; &lt;li&gt;aterro sanitário&lt;/li&gt; &lt;li&gt;doação&lt;/li&gt; &lt;li&gt;processamento das devoluções&lt;/li&gt; &lt;li&gt;reciclagem&lt;/li&gt; &lt;li&gt;reembalagem&lt;/li&gt; &lt;li&gt;remanufatura&lt;/li&gt; &lt;li&gt;revenda&lt;/li&gt; &lt;li&gt;revitalização&lt;/li&gt; &lt;li&gt;recuperação de cargas roubadas ou perdidas&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>0</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Logística Verde&lt;/b&gt;
+&lt;i&gt;Conceito&lt;/i&gt;</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>procedimentos de logística que objetivam a preservação do meio ambiente, que incluem desde a embalagem até o modal de transporte utilizado</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Logística de Pós-consumo&lt;/b&gt;
+&lt;i&gt;Características&lt;/i&gt;</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>&lt;ul&gt;
+	&lt;li&gt;favorece o retorno dos produtos após serem utilizados pelos clientes, visando: &lt;ul&gt; &lt;li&gt;reciclagem&lt;/li&gt; &lt;li&gt;reutilização ou&lt;/li&gt; &lt;li&gt;descarte apropriado&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+	&lt;li&gt;&lt;b&gt;motivação:&lt;/b&gt; &lt;ul&gt; &lt;li&gt;quantidade de materiais descartados pela sociedade desde o século XX até os dias de hoje &lt;ul&gt; &lt;li&gt;Diminuilção do ciclo de vida dos produtos&lt;/li&gt; &lt;/ul&gt; &lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+	&lt;li&gt;destinos para um produto após descarte: &lt;ul&gt; &lt;li&gt;local seguro (aterro sanitário)&lt;/li&gt; &lt;li&gt;local não seguro&lt;/li&gt; &lt;li&gt;Reciclagem&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Conhecimentos Específicos</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Logística</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;Logística de Pós-venda&lt;/b&gt;
+&lt;i&gt;Características&lt;/i&gt;</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>&lt;b&gt;uma das suas preocupações-chave: &lt;/b&gt;&lt;ul&gt; &lt;li&gt;criar um canal acessível para clientes retornarem &lt;b&gt;produtos&lt;/b&gt;. &lt;ul&gt; &lt;li&gt;defeitos de fabricação ou&lt;/li&gt; &lt;li&gt;erros no pedido&lt;/li&gt; &lt;/ul&gt;&lt;/li&gt; &lt;/ul&gt;</t>
+        </is>
+      </c>
+      <c r="F83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>